<commit_message>
Murphy did some css stuff
</commit_message>
<xml_diff>
--- a/MatchTA_UI/public/templates/example1.xlsx
+++ b/MatchTA_UI/public/templates/example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/768b4079c1f233a9/MatchTA/MatchTA_UI/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_7C39ABFFF30F9C464A3C34905030634A5738539B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA58F09E-161B-4C83-8282-79185CBDFDB7}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_7C39ABFFF30F9C464A3C34905030634A5738539B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D22C49D-5C4B-4F0C-9946-083A1F12AFC3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Headcount</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>0.5 or 1</t>
+  </si>
+  <si>
+    <t>Grad Level</t>
+  </si>
+  <si>
+    <t>Ph.D. Student or M.S. Student</t>
   </si>
 </sst>
 </file>
@@ -146,6 +152,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,60 +445,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="189.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="179.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="189.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>